<commit_message>
added time series column to schema
</commit_message>
<xml_diff>
--- a/schema/smartt_bmj_open_plus_schema.xlsx
+++ b/schema/smartt_bmj_open_plus_schema.xlsx
@@ -170,7 +170,7 @@
     <t xml:space="preserve">gender</t>
   </si>
   <si>
-    <t xml:space="preserve">BM</t>
+    <t xml:space="preserve">BMI</t>
   </si>
   <si>
     <t xml:space="preserve">bmi</t>
@@ -595,7 +595,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="160.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.53"/>
@@ -810,7 +810,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
added PtDemographic and new schema variables
</commit_message>
<xml_diff>
--- a/schema/smartt_bmj_open_plus_schema.xlsx
+++ b/schema/smartt_bmj_open_plus_schema.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="170">
   <si>
     <t xml:space="preserve">Feature Category</t>
   </si>
@@ -143,6 +143,9 @@
     <t xml:space="preserve">Possibly derived</t>
   </si>
   <si>
+    <t xml:space="preserve">Time Series</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pacmed ontology </t>
   </si>
   <si>
@@ -177,6 +180,66 @@
   </si>
   <si>
     <t xml:space="preserve">bmi, body, index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If not recorded, use weight and height to compute (i.e. derived)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">birth, date, dob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethnicity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ethnicity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ethnic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">post, code, postcode, address, zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admit source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admit_source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admit, source, admission</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hospital Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hospital_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hospital, number</t>
   </si>
   <si>
     <t xml:space="preserve">Pao2</t>
@@ -474,8 +537,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -557,12 +621,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -590,7 +658,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="1" sqref="E11:F11 B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -807,13 +875,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11:F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.14"/>
   </cols>
@@ -843,268 +911,292 @@
       <c r="H1" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>46</v>
+      <c r="F2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>46</v>
+        <v>1</v>
+      </c>
+      <c r="F4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>56</v>
+      <c r="F5" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>58</v>
-      </c>
       <c r="C6" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>56</v>
+      <c r="F6" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>62</v>
-      </c>
       <c r="D7" s="0" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F7" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>63</v>
+      <c r="F7" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F8" s="0" t="s">
-        <v>67</v>
+      <c r="F8" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F9" s="0" t="s">
-        <v>67</v>
+      <c r="F9" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F10" s="0" t="s">
-        <v>74</v>
+      <c r="F10" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F11" s="0" t="s">
-        <v>74</v>
+      <c r="F11" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F12" s="0" t="s">
-        <v>74</v>
+      <c r="F12" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>81</v>
-      </c>
       <c r="D13" s="0" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F13" s="0" t="s">
-        <v>74</v>
+      <c r="F13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="C14" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="D14" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="I14" s="0" t="s">
         <v>84</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1118,12 +1210,15 @@
         <v>87</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="0" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1138,339 +1233,551 @@
         <v>91</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F16" s="0" t="s">
-        <v>93</v>
+      <c r="F16" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="D17" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="E17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="C18" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="C18" s="0" t="s">
-        <v>99</v>
-      </c>
       <c r="D18" s="0" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F18" s="0" t="s">
-        <v>93</v>
+      <c r="F18" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="B19" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>102</v>
-      </c>
       <c r="D19" s="0" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F19" s="0" t="s">
-        <v>93</v>
+      <c r="F19" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F20" s="0" t="s">
-        <v>93</v>
+      <c r="F20" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F21" s="0" t="s">
-        <v>93</v>
+      <c r="F21" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" s="0" t="s">
         <v>109</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="E22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="D23" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="E23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" s="0" t="s">
         <v>114</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="E23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="C24" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="C24" s="0" t="s">
-        <v>118</v>
-      </c>
       <c r="D24" s="0" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F24" s="0" t="s">
-        <v>115</v>
+      <c r="F24" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B25" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="C25" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="C25" s="0" t="s">
-        <v>121</v>
-      </c>
       <c r="D25" s="0" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F25" s="0" t="s">
-        <v>115</v>
+      <c r="F25" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="C26" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>124</v>
-      </c>
       <c r="D26" s="0" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F26" s="0" t="s">
-        <v>115</v>
+      <c r="F26" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="C27" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="C27" s="0" t="s">
-        <v>127</v>
-      </c>
       <c r="D27" s="0" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F27" s="0" t="s">
-        <v>115</v>
+      <c r="F27" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B28" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="C28" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="C28" s="0" t="s">
-        <v>130</v>
-      </c>
       <c r="D28" s="0" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>132</v>
+        <v>0</v>
+      </c>
+      <c r="F28" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>131</v>
+        <v>0</v>
+      </c>
+      <c r="F29" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30" s="0" t="s">
         <v>136</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="E30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" s="0" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>29</v>
+        <v>137</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F31" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="H31" s="0" t="s">
-        <v>143</v>
+      <c r="F31" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B33" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="C33" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="D33" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="B34" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="E32" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" s="0" t="s">
+      <c r="C34" s="0" t="s">
         <v>148</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F35" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="I35" s="0" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F36" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="I38" s="0" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>